<commit_message>
Creación de planilla para las imágenes
1. Se elimina código que no hace falta y no correspondía en el .js
2. Se crea la planilla con los enlaces a las imágenes. Será un generador de enlaces con VBA Excel.
3. Se renombra un archivo con las correspondientes equivalencias y variantes de talles y color.
</commit_message>
<xml_diff>
--- a/migracionWordPressPrestashop/COLORES-TALLES-ETC.xlsx
+++ b/migracionWordPressPrestashop/COLORES-TALLES-ETC.xlsx
@@ -187,12 +187,6 @@
     <t>EQUIVALENCIA</t>
   </si>
   <si>
-    <t>CAMUFLADO</t>
-  </si>
-  <si>
-    <t>COLOR</t>
-  </si>
-  <si>
     <t>MANO</t>
   </si>
   <si>
@@ -745,10 +739,16 @@
     <t>Multicam Negro</t>
   </si>
   <si>
-    <t>RESULTADO</t>
-  </si>
-  <si>
     <t>COLORES COMPLETO</t>
+  </si>
+  <si>
+    <t>COLOR VIEJO</t>
+  </si>
+  <si>
+    <t>DESCRIP. COLOR/CAMUFL.</t>
+  </si>
+  <si>
+    <t>CÓD. COLOR</t>
   </si>
 </sst>
 </file>
@@ -815,17 +815,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:K182" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" name="EQUIVALENCIA"/>
-    <tableColumn id="2" name="CAMUFLADO"/>
+    <tableColumn id="2" name="DESCRIP. COLOR/CAMUFL."/>
     <tableColumn id="3" name="TALLE LETRA"/>
     <tableColumn id="4" name="TALLE NUMERO"/>
-    <tableColumn id="5" name="COLOR"/>
+    <tableColumn id="5" name="COLOR VIEJO"/>
     <tableColumn id="6" name="MANO"/>
     <tableColumn id="7" name="MODELO"/>
     <tableColumn id="9" name="GRUPO"/>
     <tableColumn id="8" name="USO"/>
-    <tableColumn id="10" name="RESULTADO" dataDxfId="1"/>
+    <tableColumn id="10" name="CÓD. COLOR" dataDxfId="1"/>
     <tableColumn id="11" name="COLORES COMPLETO" dataDxfId="0">
-      <calculatedColumnFormula>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</calculatedColumnFormula>
+      <calculatedColumnFormula>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1121,9 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1131,6 +1129,7 @@
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1139,7 +1138,7 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>243</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
@@ -1148,25 +1147,25 @@
         <v>55</v>
       </c>
       <c r="E1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" t="s">
-        <v>225</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
       <c r="I1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1177,19 +1176,19 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>53</v>
@@ -1209,25 +1208,25 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K3" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>01. Pitón Gris</v>
       </c>
     </row>
@@ -1245,19 +1244,19 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K4" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>02. Pitón Beige</v>
       </c>
     </row>
@@ -1275,13 +1274,13 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K5" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>03. Beige</v>
       </c>
     </row>
@@ -1299,13 +1298,13 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K6" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>04. Woodland</v>
       </c>
     </row>
@@ -1323,13 +1322,13 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K7" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>05. Digital Desert</v>
       </c>
     </row>
@@ -1347,13 +1346,13 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K8" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>06. Verde</v>
       </c>
     </row>
@@ -1371,13 +1370,13 @@
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K9" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>07. Acu</v>
       </c>
     </row>
@@ -1398,7 +1397,7 @@
         <v>12</v>
       </c>
       <c r="K10" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>08. Multicam</v>
       </c>
     </row>
@@ -1419,7 +1418,7 @@
         <v>13</v>
       </c>
       <c r="K11" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>09. Negro</v>
       </c>
     </row>
@@ -1440,7 +1439,7 @@
         <v>14</v>
       </c>
       <c r="K12" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>10. Tri Desert</v>
       </c>
     </row>
@@ -1461,7 +1460,7 @@
         <v>15</v>
       </c>
       <c r="K13" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>11. Digital Woodland</v>
       </c>
     </row>
@@ -1479,7 +1478,7 @@
         <v>16</v>
       </c>
       <c r="K14" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>12. Pitón Verde</v>
       </c>
     </row>
@@ -1497,7 +1496,7 @@
         <v>17</v>
       </c>
       <c r="K15" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>13. Gris</v>
       </c>
     </row>
@@ -1515,7 +1514,7 @@
         <v>18</v>
       </c>
       <c r="K16" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>14. Real Tree</v>
       </c>
     </row>
@@ -1533,7 +1532,7 @@
         <v>19</v>
       </c>
       <c r="K17" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>15. Digital Tiger Woodland</v>
       </c>
     </row>
@@ -1551,7 +1550,7 @@
         <v>20</v>
       </c>
       <c r="K18" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>16. Digital Fuerza Aérea</v>
       </c>
     </row>
@@ -1569,7 +1568,7 @@
         <v>21</v>
       </c>
       <c r="K19" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>17. Digital Naval</v>
       </c>
     </row>
@@ -1587,7 +1586,7 @@
         <v>22</v>
       </c>
       <c r="K20" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>18. Azul</v>
       </c>
     </row>
@@ -1596,7 +1595,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D21">
         <v>19</v>
@@ -1605,7 +1604,7 @@
         <v>23</v>
       </c>
       <c r="K21" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>19. Camuflado</v>
       </c>
     </row>
@@ -1623,7 +1622,7 @@
         <v>24</v>
       </c>
       <c r="K22" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>20. Blanco</v>
       </c>
     </row>
@@ -1632,7 +1631,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D23">
         <v>21</v>
@@ -1641,13 +1640,13 @@
         <v>25</v>
       </c>
       <c r="K23" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>21. Multicam Negro</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -1656,1756 +1655,1756 @@
         <v>22</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K24" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>22. Rojo</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D25">
         <v>23</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K25" t="str">
-        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[CAMUFLADO]])</f>
+        <f>CONCATENATE(Tabla1[[#This Row],[EQUIVALENCIA]],". ",Tabla1[[#This Row],[DESCRIP. COLOR/CAMUFL.]])</f>
         <v>23. Digital Ruso</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>24</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28">
         <v>26</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29">
         <v>27</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30">
         <v>28</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31">
         <v>29</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D32">
         <v>30</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33">
         <v>31</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34">
         <v>32</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D35">
         <v>33</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D36">
         <v>34</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D37">
         <v>35</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D38">
         <v>36</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D39">
         <v>37</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40">
         <v>38</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D41">
         <v>39</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D42">
         <v>40</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D43">
         <v>41</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D44">
         <v>42</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D45">
         <v>43</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D46">
         <v>44</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D47">
         <v>45</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D48">
         <v>46</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D49">
         <v>47</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D50">
         <v>48</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D51">
         <v>49</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D52">
         <v>50</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D53">
         <v>51</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D54">
         <v>52</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D55">
         <v>53</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D56">
         <v>54</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D57">
         <v>55</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D58">
         <v>56</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D59">
         <v>57</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D60">
         <v>58</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D61">
         <v>59</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D62">
         <v>60</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D63">
         <v>61</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D64">
         <v>62</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D65">
         <v>63</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D66">
         <v>64</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D67">
         <v>65</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D68">
         <v>66</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D69">
         <v>67</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D70">
         <v>68</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D71">
         <v>69</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D72">
         <v>70</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D73">
         <v>71</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D74">
         <v>72</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D75">
         <v>73</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D76">
         <v>74</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D77">
         <v>75</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D78">
         <v>76</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D79">
         <v>77</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D80">
         <v>78</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D81">
         <v>79</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D82">
         <v>80</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D83">
         <v>81</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D84">
         <v>82</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D85">
         <v>83</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D86">
         <v>84</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D87">
         <v>85</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D88">
         <v>86</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D89">
         <v>87</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D90">
         <v>88</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D91">
         <v>89</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D92">
         <v>90</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D93">
         <v>91</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D94">
         <v>92</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D95">
         <v>93</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D96">
         <v>94</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D97">
         <v>95</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D98">
         <v>96</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D99">
         <v>97</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D100">
         <v>98</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D101">
         <v>99</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D102">
         <v>100</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D103">
         <v>101</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D104">
         <v>102</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D105">
         <v>103</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D106">
         <v>104</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D107">
         <v>105</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D108">
         <v>106</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D109">
         <v>107</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D110">
         <v>108</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D111">
         <v>109</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D112">
         <v>110</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D113">
         <v>111</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D114">
         <v>112</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D115">
         <v>113</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D116">
         <v>114</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D117">
         <v>115</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D118">
         <v>116</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D119">
         <v>117</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D120">
         <v>118</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D121">
         <v>119</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D122">
         <v>120</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D123">
         <v>121</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D124">
         <v>122</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D125">
         <v>123</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D126">
         <v>124</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D127">
         <v>125</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D128">
         <v>126</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D129">
         <v>127</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D130">
         <v>128</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D131">
         <v>129</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D132">
         <v>130</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D133">
         <v>131</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D134">
         <v>132</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D135">
         <v>133</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D136">
         <v>134</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D137">
         <v>135</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D138">
         <v>136</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D139">
         <v>137</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D140">
         <v>138</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D141">
         <v>139</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D142">
         <v>140</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D143">
         <v>141</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D144">
         <v>142</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D145">
         <v>143</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D146">
         <v>144</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D147">
         <v>145</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D148">
         <v>146</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D149">
         <v>147</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D150">
         <v>148</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D151">
         <v>149</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D152">
         <v>150</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D153">
         <v>151</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D154">
         <v>152</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D155">
         <v>153</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D156">
         <v>154</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D157">
         <v>155</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D158">
         <v>156</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D159">
         <v>157</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D160">
         <v>158</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D161">
         <v>159</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D162">
         <v>160</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D163">
         <v>161</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D164">
         <v>162</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D165">
         <v>163</v>
       </c>
       <c r="J165" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D166">
         <v>164</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D167">
         <v>165</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D168">
         <v>166</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D169">
         <v>167</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D170">
         <v>168</v>
       </c>
       <c r="J170" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D171">
         <v>169</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D172">
         <v>170</v>
       </c>
       <c r="J172" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D173">
         <v>171</v>
       </c>
       <c r="J173" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D174">
         <v>172</v>
       </c>
       <c r="J174" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D175">
         <v>173</v>
       </c>
       <c r="J175" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D176">
         <v>174</v>
       </c>
       <c r="J176" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D177">
         <v>175</v>
       </c>
       <c r="J177" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D178">
         <v>176</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D179">
         <v>177</v>
       </c>
       <c r="J179" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D180">
         <v>178</v>
       </c>
       <c r="J180" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D181">
         <v>179</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D182">
         <v>180</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cosas varias que no tienen sentido.
</commit_message>
<xml_diff>
--- a/migracionWordPressPrestashop/COLORES-TALLES-ETC.xlsx
+++ b/migracionWordPressPrestashop/COLORES-TALLES-ETC.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="245">
   <si>
     <t>Azul</t>
   </si>
@@ -1119,9 +1119,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1750,6 +1753,12 @@
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
       <c r="D32">
         <v>30</v>
       </c>
@@ -1761,6 +1770,12 @@
       <c r="A33" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
       <c r="D33">
         <v>31</v>
       </c>
@@ -1772,6 +1787,12 @@
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
       <c r="D34">
         <v>32</v>
       </c>
@@ -1783,6 +1804,12 @@
       <c r="A35" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
       <c r="D35">
         <v>33</v>
       </c>
@@ -1794,6 +1821,12 @@
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
       <c r="D36">
         <v>34</v>
       </c>
@@ -1805,6 +1838,12 @@
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
       <c r="D37">
         <v>35</v>
       </c>
@@ -1816,6 +1855,12 @@
       <c r="A38" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
       <c r="D38">
         <v>36</v>
       </c>
@@ -1827,6 +1872,12 @@
       <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
       <c r="D39">
         <v>37</v>
       </c>
@@ -1838,6 +1889,12 @@
       <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
       <c r="D40">
         <v>38</v>
       </c>
@@ -1849,6 +1906,12 @@
       <c r="A41" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
       <c r="D41">
         <v>39</v>
       </c>
@@ -2410,6 +2473,12 @@
       <c r="A92" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>41</v>
+      </c>
       <c r="D92">
         <v>90</v>
       </c>
@@ -2421,6 +2490,12 @@
       <c r="A93" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>42</v>
+      </c>
       <c r="D93">
         <v>91</v>
       </c>
@@ -2432,6 +2507,12 @@
       <c r="A94" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" t="s">
+        <v>43</v>
+      </c>
       <c r="D94">
         <v>92</v>
       </c>
@@ -2443,6 +2524,12 @@
       <c r="A95" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>44</v>
+      </c>
       <c r="D95">
         <v>93</v>
       </c>
@@ -2454,6 +2541,12 @@
       <c r="A96" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="B96" t="s">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>45</v>
+      </c>
       <c r="D96">
         <v>94</v>
       </c>
@@ -2465,6 +2558,12 @@
       <c r="A97" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>46</v>
+      </c>
       <c r="D97">
         <v>95</v>
       </c>
@@ -2476,6 +2575,12 @@
       <c r="A98" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>47</v>
+      </c>
       <c r="D98">
         <v>96</v>
       </c>
@@ -2487,6 +2592,12 @@
       <c r="A99" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>48</v>
+      </c>
       <c r="D99">
         <v>97</v>
       </c>
@@ -2498,6 +2609,12 @@
       <c r="A100" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>49</v>
+      </c>
       <c r="D100">
         <v>98</v>
       </c>
@@ -2508,6 +2625,12 @@
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>50</v>
       </c>
       <c r="D101">
         <v>99</v>

</xml_diff>